<commit_message>
work on prep for removal
Worked on class-less assets and classes to remove
</commit_message>
<xml_diff>
--- a/Avantis Mapping/SPARQL_superclass.xlsx
+++ b/Avantis Mapping/SPARQL_superclass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medney\Documents\GitHub\TWONTO\Avantis Mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E92C92C-CDF7-4F6C-BBEE-669BD72CD4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16D84FD-BB73-48DA-B739-55D9128C163C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{716C0CF8-2E33-46F2-BE6F-578AC5702A19}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{716C0CF8-2E33-46F2-BE6F-578AC5702A19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,13 +65,13 @@
 }</t>
   </si>
   <si>
-    <t>instrument gauge or display</t>
-  </si>
-  <si>
-    <t>cable segment</t>
-  </si>
-  <si>
-    <t>air duct segment</t>
+    <t>http://www.toronto.ca/TWONTO#air_duct_segment</t>
+  </si>
+  <si>
+    <t>http://www.toronto.ca/TWONTO#cable_segment</t>
+  </si>
+  <si>
+    <t>http://www.toronto.ca/TWONTO#instrument_gauge_or_display</t>
   </si>
 </sst>
 </file>
@@ -494,21 +494,21 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A3" sqref="A3:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="61.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="165" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -516,15 +516,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -532,12 +532,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>